<commit_message>
more function in the class
More functions added into the class, such as
1. switching mode
2. set/get mode parameters.
3. and simple error handling.
</commit_message>
<xml_diff>
--- a/Lens Driver V4 Communication Protocol incl. example.xlsx
+++ b/Lens Driver V4 Communication Protocol incl. example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="255" windowWidth="3765" windowHeight="9270" tabRatio="784" activeTab="2"/>
+    <workbookView xWindow="4650" yWindow="255" windowWidth="3765" windowHeight="9270" tabRatio="784" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="8" r:id="rId1"/>
@@ -5933,42 +5933,7 @@
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="192">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="175">
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
@@ -6015,40 +5980,8 @@
     <dxf>
       <fill>
         <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
           <fgColor theme="0" tint="-4.9989318521683403E-2"/>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6113,76 +6046,9 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill patternType="lightDown">
           <fgColor theme="0" tint="-4.9989318521683403E-2"/>
           <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-0.24994659260841701"/>
-          <bgColor theme="6" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7421,14 +7287,6 @@
         <patternFill patternType="lightDown">
           <fgColor theme="0" tint="-0.24994659260841701"/>
           <bgColor theme="6" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightDown">
-          <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -13160,11 +13018,11 @@
   <dimension ref="B1:Z64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
       <selection pane="topRight" activeCell="D25" sqref="D25"/>
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15805,7 +15663,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="37" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:26" s="121" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B37" s="112" t="s">
         <v>348</v>
       </c>
@@ -15874,7 +15732,7 @@
       </c>
       <c r="Z37" s="127"/>
     </row>
-    <row r="38" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:26" s="121" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="112" t="s">
         <v>348</v>
       </c>
@@ -16152,7 +16010,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="42" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:26" s="121" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B42" s="112" t="s">
         <v>348</v>
       </c>
@@ -16227,7 +16085,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="43" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:26" s="121" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="B43" s="112" t="s">
         <v>348</v>
       </c>
@@ -16461,757 +16319,757 @@
     <mergeCell ref="P1:Y1"/>
   </mergeCells>
   <conditionalFormatting sqref="X11:Z11 Z6:Z7 X3:Z5 I47 Y40:Z40 D38:H38 D8:G8 D3 U31:V31 M39:Z39 D40:O40 J38:Z38 D4:W7 I8:Z8 D11:V12 F3:W3 D31:N31 Q40:W40 D39:K39 D28:O28 D42:Z42">
-    <cfRule type="expression" dxfId="191" priority="366">
+    <cfRule type="expression" dxfId="174" priority="366">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:W10 D9:T10 D29:Y29 D37:V37 D30:Z30">
-    <cfRule type="expression" dxfId="190" priority="365">
+    <cfRule type="expression" dxfId="173" priority="365">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X9:Z10">
-    <cfRule type="expression" dxfId="189" priority="364">
+    <cfRule type="expression" dxfId="172" priority="364">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y6:Y7">
-    <cfRule type="expression" dxfId="188" priority="363">
+    <cfRule type="expression" dxfId="171" priority="363">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40">
-    <cfRule type="expression" dxfId="187" priority="359">
+    <cfRule type="expression" dxfId="170" priority="359">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X40">
-    <cfRule type="expression" dxfId="186" priority="358">
+    <cfRule type="expression" dxfId="169" priority="358">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X6">
-    <cfRule type="expression" dxfId="185" priority="352">
+    <cfRule type="expression" dxfId="168" priority="352">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X7">
-    <cfRule type="expression" dxfId="184" priority="351">
+    <cfRule type="expression" dxfId="167" priority="351">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W11">
-    <cfRule type="expression" dxfId="183" priority="369">
+    <cfRule type="expression" dxfId="166" priority="369">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="expression" dxfId="182" priority="333">
+    <cfRule type="expression" dxfId="165" priority="333">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X37:Y37">
-    <cfRule type="expression" dxfId="180" priority="322">
+    <cfRule type="expression" dxfId="164" priority="322">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W37">
-    <cfRule type="expression" dxfId="179" priority="323">
+    <cfRule type="expression" dxfId="163" priority="323">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38">
-    <cfRule type="expression" dxfId="178" priority="320">
+    <cfRule type="expression" dxfId="162" priority="320">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39">
-    <cfRule type="expression" dxfId="177" priority="318">
+    <cfRule type="expression" dxfId="161" priority="318">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X12:Y12">
-    <cfRule type="expression" dxfId="176" priority="315">
+    <cfRule type="expression" dxfId="160" priority="315">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z12">
-    <cfRule type="expression" dxfId="175" priority="316">
+    <cfRule type="expression" dxfId="159" priority="316">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W12">
-    <cfRule type="expression" dxfId="174" priority="317">
+    <cfRule type="expression" dxfId="158" priority="317">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X31">
-    <cfRule type="expression" dxfId="173" priority="216">
+    <cfRule type="expression" dxfId="157" priority="216">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z31">
-    <cfRule type="expression" dxfId="172" priority="214">
+    <cfRule type="expression" dxfId="156" priority="214">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O31">
-    <cfRule type="expression" dxfId="171" priority="213">
+    <cfRule type="expression" dxfId="155" priority="213">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="170" priority="163">
+    <cfRule type="expression" dxfId="154" priority="163">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28:Y28">
-    <cfRule type="expression" dxfId="169" priority="158">
+    <cfRule type="expression" dxfId="153" priority="158">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z28">
-    <cfRule type="expression" dxfId="168" priority="157">
+    <cfRule type="expression" dxfId="152" priority="157">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z29">
-    <cfRule type="expression" dxfId="167" priority="152">
+    <cfRule type="expression" dxfId="151" priority="152">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:Z12 B28:Z31 B37:Z40 B42:Z42 B46:Z164">
-    <cfRule type="expression" dxfId="166" priority="425">
+    <cfRule type="expression" dxfId="150" priority="425">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="165" priority="426">
+    <cfRule type="expression" dxfId="149" priority="426">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="164" priority="427">
+    <cfRule type="expression" dxfId="148" priority="427">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="163" priority="428">
+    <cfRule type="expression" dxfId="147" priority="428">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z13:Z14 D13:W14">
-    <cfRule type="expression" dxfId="162" priority="143">
+    <cfRule type="expression" dxfId="146" priority="143">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y13:Y14">
-    <cfRule type="expression" dxfId="161" priority="142">
+    <cfRule type="expression" dxfId="145" priority="142">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X13:X14">
-    <cfRule type="expression" dxfId="160" priority="141">
+    <cfRule type="expression" dxfId="144" priority="141">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:Z14">
-    <cfRule type="expression" dxfId="159" priority="144">
+    <cfRule type="expression" dxfId="143" priority="144">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="158" priority="145">
+    <cfRule type="expression" dxfId="142" priority="145">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="157" priority="146">
+    <cfRule type="expression" dxfId="141" priority="146">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="156" priority="147">
+    <cfRule type="expression" dxfId="140" priority="147">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15:V15">
-    <cfRule type="expression" dxfId="155" priority="136">
+    <cfRule type="expression" dxfId="139" priority="136">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X15:Y15">
-    <cfRule type="expression" dxfId="154" priority="133">
+    <cfRule type="expression" dxfId="138" priority="133">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z15">
-    <cfRule type="expression" dxfId="153" priority="134">
+    <cfRule type="expression" dxfId="137" priority="134">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W15">
-    <cfRule type="expression" dxfId="152" priority="135">
+    <cfRule type="expression" dxfId="136" priority="135">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15:Z15">
-    <cfRule type="expression" dxfId="151" priority="137">
+    <cfRule type="expression" dxfId="135" priority="137">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="150" priority="138">
+    <cfRule type="expression" dxfId="134" priority="138">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="149" priority="139">
+    <cfRule type="expression" dxfId="133" priority="139">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="148" priority="140">
+    <cfRule type="expression" dxfId="132" priority="140">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z16 D16:W16">
-    <cfRule type="expression" dxfId="147" priority="128">
+    <cfRule type="expression" dxfId="131" priority="128">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y16">
-    <cfRule type="expression" dxfId="146" priority="127">
+    <cfRule type="expression" dxfId="130" priority="127">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X16">
-    <cfRule type="expression" dxfId="145" priority="126">
+    <cfRule type="expression" dxfId="129" priority="126">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:Z16">
-    <cfRule type="expression" dxfId="144" priority="129">
+    <cfRule type="expression" dxfId="128" priority="129">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="143" priority="130">
+    <cfRule type="expression" dxfId="127" priority="130">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="142" priority="131">
+    <cfRule type="expression" dxfId="126" priority="131">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="141" priority="132">
+    <cfRule type="expression" dxfId="125" priority="132">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17:V18">
-    <cfRule type="expression" dxfId="140" priority="121">
+    <cfRule type="expression" dxfId="124" priority="121">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X17:Y18">
-    <cfRule type="expression" dxfId="139" priority="118">
+    <cfRule type="expression" dxfId="123" priority="118">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17:Z18">
-    <cfRule type="expression" dxfId="138" priority="119">
+    <cfRule type="expression" dxfId="122" priority="119">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W17:W18">
-    <cfRule type="expression" dxfId="137" priority="120">
+    <cfRule type="expression" dxfId="121" priority="120">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17:Z18">
-    <cfRule type="expression" dxfId="136" priority="122">
+    <cfRule type="expression" dxfId="120" priority="122">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="123">
+    <cfRule type="expression" dxfId="119" priority="123">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="124">
+    <cfRule type="expression" dxfId="118" priority="124">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="125">
+    <cfRule type="expression" dxfId="117" priority="125">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19:V19">
-    <cfRule type="expression" dxfId="132" priority="113">
+    <cfRule type="expression" dxfId="116" priority="113">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X19:Y19">
-    <cfRule type="expression" dxfId="131" priority="110">
+    <cfRule type="expression" dxfId="115" priority="110">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z19">
-    <cfRule type="expression" dxfId="130" priority="111">
+    <cfRule type="expression" dxfId="114" priority="111">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W19">
-    <cfRule type="expression" dxfId="129" priority="112">
+    <cfRule type="expression" dxfId="113" priority="112">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:Z19">
-    <cfRule type="expression" dxfId="128" priority="114">
+    <cfRule type="expression" dxfId="112" priority="114">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="115">
+    <cfRule type="expression" dxfId="111" priority="115">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="126" priority="116">
+    <cfRule type="expression" dxfId="110" priority="116">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="117">
+    <cfRule type="expression" dxfId="109" priority="117">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20:V20">
-    <cfRule type="expression" dxfId="124" priority="105">
+    <cfRule type="expression" dxfId="108" priority="105">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X20:Y20">
-    <cfRule type="expression" dxfId="123" priority="102">
+    <cfRule type="expression" dxfId="107" priority="102">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z20">
-    <cfRule type="expression" dxfId="122" priority="103">
+    <cfRule type="expression" dxfId="106" priority="103">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W20">
-    <cfRule type="expression" dxfId="121" priority="104">
+    <cfRule type="expression" dxfId="105" priority="104">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20:Z20">
-    <cfRule type="expression" dxfId="120" priority="106">
+    <cfRule type="expression" dxfId="104" priority="106">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="107">
+    <cfRule type="expression" dxfId="103" priority="107">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="108">
+    <cfRule type="expression" dxfId="102" priority="108">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="109">
+    <cfRule type="expression" dxfId="101" priority="109">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:V21">
-    <cfRule type="expression" dxfId="116" priority="97">
+    <cfRule type="expression" dxfId="100" priority="97">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X21:Y21">
-    <cfRule type="expression" dxfId="115" priority="94">
+    <cfRule type="expression" dxfId="99" priority="94">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z21">
-    <cfRule type="expression" dxfId="114" priority="95">
+    <cfRule type="expression" dxfId="98" priority="95">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W21">
-    <cfRule type="expression" dxfId="113" priority="96">
+    <cfRule type="expression" dxfId="97" priority="96">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:Z21">
-    <cfRule type="expression" dxfId="112" priority="98">
+    <cfRule type="expression" dxfId="96" priority="98">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="99">
+    <cfRule type="expression" dxfId="95" priority="99">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="100">
+    <cfRule type="expression" dxfId="94" priority="100">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="101">
+    <cfRule type="expression" dxfId="93" priority="101">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32:V33">
-    <cfRule type="expression" dxfId="108" priority="89">
+    <cfRule type="expression" dxfId="92" priority="89">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X32:Y33">
-    <cfRule type="expression" dxfId="107" priority="86">
+    <cfRule type="expression" dxfId="91" priority="86">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z32:Z33">
-    <cfRule type="expression" dxfId="106" priority="87">
+    <cfRule type="expression" dxfId="90" priority="87">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W32:W33">
-    <cfRule type="expression" dxfId="105" priority="88">
+    <cfRule type="expression" dxfId="89" priority="88">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:Z33">
-    <cfRule type="expression" dxfId="104" priority="90">
+    <cfRule type="expression" dxfId="88" priority="90">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="91">
+    <cfRule type="expression" dxfId="87" priority="91">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="92">
+    <cfRule type="expression" dxfId="86" priority="92">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="93">
+    <cfRule type="expression" dxfId="85" priority="93">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z34:Z36 D34:W36">
-    <cfRule type="expression" dxfId="100" priority="81">
+    <cfRule type="expression" dxfId="84" priority="81">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y34:Y36">
-    <cfRule type="expression" dxfId="99" priority="80">
+    <cfRule type="expression" dxfId="83" priority="80">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X34:X36">
-    <cfRule type="expression" dxfId="98" priority="79">
+    <cfRule type="expression" dxfId="82" priority="79">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:Z36">
-    <cfRule type="expression" dxfId="97" priority="82">
+    <cfRule type="expression" dxfId="81" priority="82">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="83">
+    <cfRule type="expression" dxfId="80" priority="83">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="84">
+    <cfRule type="expression" dxfId="79" priority="84">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="85">
+    <cfRule type="expression" dxfId="78" priority="85">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:V42">
-    <cfRule type="expression" dxfId="93" priority="74">
+    <cfRule type="expression" dxfId="77" priority="74">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X37:Y42">
-    <cfRule type="expression" dxfId="92" priority="71">
+    <cfRule type="expression" dxfId="76" priority="71">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z37:Z42">
-    <cfRule type="expression" dxfId="91" priority="72">
+    <cfRule type="expression" dxfId="75" priority="72">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W37:W42">
-    <cfRule type="expression" dxfId="90" priority="73">
+    <cfRule type="expression" dxfId="74" priority="73">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37:Z42">
-    <cfRule type="expression" dxfId="89" priority="75">
+    <cfRule type="expression" dxfId="73" priority="75">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="76">
+    <cfRule type="expression" dxfId="72" priority="76">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="77">
+    <cfRule type="expression" dxfId="71" priority="77">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="78">
+    <cfRule type="expression" dxfId="70" priority="78">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:V43">
-    <cfRule type="expression" dxfId="85" priority="66">
+    <cfRule type="expression" dxfId="69" priority="66">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X43:Y43">
-    <cfRule type="expression" dxfId="84" priority="64">
+    <cfRule type="expression" dxfId="68" priority="64">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43">
-    <cfRule type="expression" dxfId="83" priority="65">
+    <cfRule type="expression" dxfId="67" priority="65">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:Z43">
-    <cfRule type="expression" dxfId="82" priority="67">
+    <cfRule type="expression" dxfId="66" priority="67">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="68">
+    <cfRule type="expression" dxfId="65" priority="68">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="69">
+    <cfRule type="expression" dxfId="64" priority="69">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="70">
+    <cfRule type="expression" dxfId="63" priority="70">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43:V43">
-    <cfRule type="expression" dxfId="78" priority="59">
+    <cfRule type="expression" dxfId="62" priority="59">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X43:Y43">
-    <cfRule type="expression" dxfId="77" priority="56">
+    <cfRule type="expression" dxfId="61" priority="56">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z43">
-    <cfRule type="expression" dxfId="76" priority="57">
+    <cfRule type="expression" dxfId="60" priority="57">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W43">
-    <cfRule type="expression" dxfId="75" priority="58">
+    <cfRule type="expression" dxfId="59" priority="58">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43:Z43">
-    <cfRule type="expression" dxfId="74" priority="60">
+    <cfRule type="expression" dxfId="58" priority="60">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="61">
+    <cfRule type="expression" dxfId="57" priority="61">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="62">
+    <cfRule type="expression" dxfId="56" priority="62">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="63">
+    <cfRule type="expression" dxfId="55" priority="63">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44:Z45 D44:W45">
-    <cfRule type="expression" dxfId="70" priority="51">
+    <cfRule type="expression" dxfId="54" priority="51">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y44:Y45">
-    <cfRule type="expression" dxfId="69" priority="50">
+    <cfRule type="expression" dxfId="53" priority="50">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X44:X45">
-    <cfRule type="expression" dxfId="68" priority="49">
+    <cfRule type="expression" dxfId="52" priority="49">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44:Z45">
-    <cfRule type="expression" dxfId="67" priority="52">
+    <cfRule type="expression" dxfId="51" priority="52">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="53">
+    <cfRule type="expression" dxfId="50" priority="53">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="54">
+    <cfRule type="expression" dxfId="49" priority="54">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="55">
+    <cfRule type="expression" dxfId="48" priority="55">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:V22">
-    <cfRule type="expression" dxfId="63" priority="44">
+    <cfRule type="expression" dxfId="47" priority="44">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X22:Y22">
-    <cfRule type="expression" dxfId="62" priority="41">
+    <cfRule type="expression" dxfId="46" priority="41">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z22">
-    <cfRule type="expression" dxfId="61" priority="42">
+    <cfRule type="expression" dxfId="45" priority="42">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W22">
-    <cfRule type="expression" dxfId="60" priority="43">
+    <cfRule type="expression" dxfId="44" priority="43">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22:Z22">
-    <cfRule type="expression" dxfId="59" priority="45">
+    <cfRule type="expression" dxfId="43" priority="45">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="46">
+    <cfRule type="expression" dxfId="42" priority="46">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="47">
+    <cfRule type="expression" dxfId="41" priority="47">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="48">
+    <cfRule type="expression" dxfId="40" priority="48">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:V24">
-    <cfRule type="expression" dxfId="55" priority="36">
+    <cfRule type="expression" dxfId="39" priority="36">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X24:Y24">
-    <cfRule type="expression" dxfId="54" priority="33">
+    <cfRule type="expression" dxfId="38" priority="33">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z24">
-    <cfRule type="expression" dxfId="53" priority="34">
+    <cfRule type="expression" dxfId="37" priority="34">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W24">
-    <cfRule type="expression" dxfId="52" priority="35">
+    <cfRule type="expression" dxfId="36" priority="35">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:Z24">
-    <cfRule type="expression" dxfId="51" priority="37">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="38">
+    <cfRule type="expression" dxfId="34" priority="38">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="39">
+    <cfRule type="expression" dxfId="33" priority="39">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="40">
+    <cfRule type="expression" dxfId="32" priority="40">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:V25">
-    <cfRule type="expression" dxfId="47" priority="28">
+    <cfRule type="expression" dxfId="31" priority="28">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X25:Y25">
-    <cfRule type="expression" dxfId="46" priority="25">
+    <cfRule type="expression" dxfId="30" priority="25">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="expression" dxfId="45" priority="26">
+    <cfRule type="expression" dxfId="29" priority="26">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25">
-    <cfRule type="expression" dxfId="44" priority="27">
+    <cfRule type="expression" dxfId="28" priority="27">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:Z25">
-    <cfRule type="expression" dxfId="43" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="30">
+    <cfRule type="expression" dxfId="26" priority="30">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="31">
+    <cfRule type="expression" dxfId="25" priority="31">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="32">
+    <cfRule type="expression" dxfId="24" priority="32">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:V26">
-    <cfRule type="expression" dxfId="39" priority="20">
+    <cfRule type="expression" dxfId="23" priority="20">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X26:Y26">
-    <cfRule type="expression" dxfId="38" priority="17">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z26">
-    <cfRule type="expression" dxfId="37" priority="18">
+    <cfRule type="expression" dxfId="21" priority="18">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W26">
-    <cfRule type="expression" dxfId="36" priority="19">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:Z26">
-    <cfRule type="expression" dxfId="35" priority="21">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="22">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="23">
+    <cfRule type="expression" dxfId="17" priority="23">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="24">
+    <cfRule type="expression" dxfId="16" priority="24">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:V27">
-    <cfRule type="expression" dxfId="31" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X27:Y27">
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z27">
-    <cfRule type="expression" dxfId="27" priority="10">
+    <cfRule type="expression" dxfId="13" priority="10">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W27">
-    <cfRule type="expression" dxfId="25" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:Z27">
-    <cfRule type="expression" dxfId="23" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="10" priority="14">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="15">
+    <cfRule type="expression" dxfId="9" priority="15">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="16">
+    <cfRule type="expression" dxfId="8" priority="16">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:V23">
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23:Y23">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W23">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:Z23">
-    <cfRule type="expression" dxfId="7" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>IF(#REF!="DEPRECATED",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>IF(#REF!="NEW",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>IF(#REF!="ACTIVE",1,0)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>IF(#REF!="Yes",1,0)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
de-bug of the Modes
The information on the manual are in-correct. How the class is able to
get feedback of the Mode-frequency, lower current and upper current.
When turnning off the lens. it will be swithed to current mode and
current = 0. Otherwise it will continue its mode even it is Closed.
change and feedback of the mode-frequency, mode Current etc is only
possible when in sin/rect/trianglar mode.
</commit_message>
<xml_diff>
--- a/Lens Driver V4 Communication Protocol incl. example.xlsx
+++ b/Lens Driver V4 Communication Protocol incl. example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="255" windowWidth="3765" windowHeight="9270" tabRatio="784" activeTab="2"/>
+    <workbookView xWindow="5580" yWindow="255" windowWidth="3765" windowHeight="9270" tabRatio="784" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="533">
   <si>
     <t>Name</t>
   </si>
@@ -4914,6 +4914,9 @@
   </si>
   <si>
     <t>PUA&lt;encoded upper swing limit&gt;&lt;0&gt;&lt;0&gt;&lt;CRC&gt;\r\n</t>
+  </si>
+  <si>
+    <t>"MP"</t>
   </si>
 </sst>
 </file>
@@ -13018,11 +13021,11 @@
   <dimension ref="B1:Z64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="I42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="Q41" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D25" sqref="D25"/>
       <selection pane="topRight" activeCell="D25" sqref="D25"/>
       <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
-      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14546,7 +14549,7 @@
       </c>
       <c r="Z21" s="127"/>
     </row>
-    <row r="22" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" s="121" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B22" s="112" t="s">
         <v>347</v>
       </c>
@@ -14623,7 +14626,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" s="121" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B23" s="112" t="s">
         <v>347</v>
       </c>
@@ -14668,7 +14671,7 @@
         <v>276</v>
       </c>
       <c r="Q23" s="123" t="s">
-        <v>8</v>
+        <v>532</v>
       </c>
       <c r="R23" s="124" t="s">
         <v>9</v>
@@ -14775,7 +14778,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:26" s="121" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B25" s="112" t="s">
         <v>347</v>
       </c>
@@ -14820,7 +14823,7 @@
         <v>276</v>
       </c>
       <c r="Q25" s="123" t="s">
-        <v>8</v>
+        <v>532</v>
       </c>
       <c r="R25" s="124" t="s">
         <v>10</v>
@@ -14927,7 +14930,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="27" spans="2:26" s="121" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:26" s="121" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B27" s="112" t="s">
         <v>347</v>
       </c>
@@ -14972,7 +14975,7 @@
         <v>276</v>
       </c>
       <c r="Q27" s="123" t="s">
-        <v>8</v>
+        <v>532</v>
       </c>
       <c r="R27" s="124" t="s">
         <v>15</v>

</xml_diff>